<commit_message>
Improving Code Coverage and Cleaning Legacy Codes
</commit_message>
<xml_diff>
--- a/Congestion-Tax-Calculator-Net-Core-Solution/Code Metrics.xlsx
+++ b/Congestion-Tax-Calculator-Net-Core-Solution/Code Metrics.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Check\Backend Technical Test\Congestion-Tax-Calculator-Net-Core-Solution\netcore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Check\Assignments\Congestion-Tax-Calculator-Net-Core-Solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A32ABAE-1986-4450-A69C-6300C86FB5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAF6FF60-1B0C-4A7F-BC82-389243D2F327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="1200" windowWidth="20910" windowHeight="11835" xr2:uid="{81B13782-A204-4AE5-AC53-82E87B03A453}"/>
+    <workbookView xWindow="4830" yWindow="1200" windowWidth="20910" windowHeight="11835" xr2:uid="{77E06B72-5CC3-4482-A303-60BB3C32AD06}"/>
   </bookViews>
   <sheets>
-    <sheet name="Code Metrics" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Code Metrics'!$A$1:$K$160</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$160</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -831,7 +831,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18236B7C-EAD0-4A33-BAC5-30A8716B0C5A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93986562-B447-4A8F-B125-FC2B30B194DB}">
   <dimension ref="A1:K160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -903,19 +903,19 @@
         <v>82</v>
       </c>
       <c r="G2">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
       <c r="I2">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J2">
-        <v>1670</v>
+        <v>1679</v>
       </c>
       <c r="K2">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -944,10 +944,10 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="K3">
         <v>41</v>
@@ -1046,10 +1046,10 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J6">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="K6">
         <v>37</v>
@@ -1564,19 +1564,19 @@
         <v>73</v>
       </c>
       <c r="G22">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J22">
-        <v>696</v>
+        <v>683</v>
       </c>
       <c r="K22">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1605,10 +1605,10 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J23">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="K23">
         <v>15</v>
@@ -1704,7 +1704,7 @@
         <v>4</v>
       </c>
       <c r="J26">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="K26">
         <v>14</v>
@@ -1739,7 +1739,7 @@
         <v>11</v>
       </c>
       <c r="J27">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K27">
         <v>18</v>
@@ -1835,7 +1835,7 @@
         <v>10</v>
       </c>
       <c r="J30">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K30">
         <v>17</v>
@@ -1867,10 +1867,10 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J31">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K31">
         <v>19</v>
@@ -1902,7 +1902,7 @@
         <v>3</v>
       </c>
       <c r="J32">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K32">
         <v>14</v>
@@ -1934,7 +1934,7 @@
         <v>2</v>
       </c>
       <c r="J33">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K33">
         <v>5</v>
@@ -1957,22 +1957,22 @@
         <v>13</v>
       </c>
       <c r="F34">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G34">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J34">
         <v>75</v>
       </c>
       <c r="K34">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1992,19 +1992,19 @@
         <v>38</v>
       </c>
       <c r="F35">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G35">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J35">
         <v>31</v>
       </c>
       <c r="K35">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2068,7 +2068,7 @@
         <v>13</v>
       </c>
       <c r="J37">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K37">
         <v>13</v>
@@ -2292,7 +2292,7 @@
         <v>4</v>
       </c>
       <c r="J44">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K44">
         <v>6</v>
@@ -2897,7 +2897,7 @@
         <v>13</v>
       </c>
       <c r="F63">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G63">
         <v>2</v>
@@ -2906,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="I63">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J63">
         <v>64</v>
@@ -2976,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="J65">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K65">
         <v>2</v>
@@ -3040,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="J67">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -3497,7 +3497,7 @@
         <v>3</v>
       </c>
       <c r="J81">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="K81">
         <v>1</v>
@@ -3800,7 +3800,7 @@
         <v>1</v>
       </c>
       <c r="J90">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -3832,7 +3832,7 @@
         <v>1</v>
       </c>
       <c r="J91">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K91">
         <v>1</v>
@@ -4376,7 +4376,7 @@
         <v>87</v>
       </c>
       <c r="G108">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H108">
         <v>1</v>
@@ -4385,10 +4385,10 @@
         <v>16</v>
       </c>
       <c r="J108">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="K108">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -4417,10 +4417,10 @@
         <v>1</v>
       </c>
       <c r="I109">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J109">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K109">
         <v>2</v>
@@ -4507,10 +4507,10 @@
         <v>13</v>
       </c>
       <c r="F112">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G112">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H112">
         <v>1</v>
@@ -4519,10 +4519,10 @@
         <v>9</v>
       </c>
       <c r="J112">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="K112">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
@@ -4734,19 +4734,19 @@
         <v>111</v>
       </c>
       <c r="F119">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="G119">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I119">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J119">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K119">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -4798,19 +4798,19 @@
         <v>113</v>
       </c>
       <c r="F121">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="G121">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I121">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J121">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K121">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
@@ -5310,19 +5310,19 @@
         <v>98</v>
       </c>
       <c r="F137">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="G137">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I137">
         <v>1</v>
       </c>
       <c r="J137">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="K137">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
@@ -5383,10 +5383,10 @@
         <v>1</v>
       </c>
       <c r="I139">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J139">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K139">
         <v>1</v>
@@ -5546,10 +5546,10 @@
         <v>3</v>
       </c>
       <c r="I144">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J144">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K144">
         <v>33</v>
@@ -5584,7 +5584,7 @@
         <v>14</v>
       </c>
       <c r="J145">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K145">
         <v>8</v>
@@ -5680,7 +5680,7 @@
         <v>13</v>
       </c>
       <c r="J148">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K148">
         <v>7</v>
@@ -5712,10 +5712,10 @@
         <v>3</v>
       </c>
       <c r="I149">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J149">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K149">
         <v>8</v>
@@ -5779,10 +5779,10 @@
         <v>1</v>
       </c>
       <c r="I151">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J151">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K151">
         <v>2</v>
@@ -6086,7 +6086,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K160" xr:uid="{18236B7C-EAD0-4A33-BAC5-30A8716B0C5A}"/>
+  <autoFilter ref="A1:K160" xr:uid="{93986562-B447-4A8F-B125-FC2B30B194DB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Dynamic Holiday Calculator and Improving Code Coverages and Metrics
</commit_message>
<xml_diff>
--- a/Congestion-Tax-Calculator-Net-Core-Solution/Code Metrics.xlsx
+++ b/Congestion-Tax-Calculator-Net-Core-Solution/Code Metrics.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Check\Assignments\Congestion-Tax-Calculator-Net-Core-Solution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Check\Backend Technical Test\Congestion-Tax-Calculator-Net-Core-Solution\netcore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAF6FF60-1B0C-4A7F-BC82-389243D2F327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A32ABAE-1986-4450-A69C-6300C86FB5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="1200" windowWidth="20910" windowHeight="11835" xr2:uid="{77E06B72-5CC3-4482-A303-60BB3C32AD06}"/>
+    <workbookView xWindow="4830" yWindow="1200" windowWidth="20910" windowHeight="11835" xr2:uid="{81B13782-A204-4AE5-AC53-82E87B03A453}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Code Metrics" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$160</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Code Metrics'!$A$1:$K$160</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -831,7 +831,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93986562-B447-4A8F-B125-FC2B30B194DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18236B7C-EAD0-4A33-BAC5-30A8716B0C5A}">
   <dimension ref="A1:K160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -903,19 +903,19 @@
         <v>82</v>
       </c>
       <c r="G2">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
       <c r="I2">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J2">
-        <v>1679</v>
+        <v>1670</v>
       </c>
       <c r="K2">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -944,10 +944,10 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="K3">
         <v>41</v>
@@ -1046,10 +1046,10 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J6">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="K6">
         <v>37</v>
@@ -1564,19 +1564,19 @@
         <v>73</v>
       </c>
       <c r="G22">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J22">
-        <v>683</v>
+        <v>696</v>
       </c>
       <c r="K22">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1605,10 +1605,10 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J23">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="K23">
         <v>15</v>
@@ -1704,7 +1704,7 @@
         <v>4</v>
       </c>
       <c r="J26">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="K26">
         <v>14</v>
@@ -1739,7 +1739,7 @@
         <v>11</v>
       </c>
       <c r="J27">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="K27">
         <v>18</v>
@@ -1835,7 +1835,7 @@
         <v>10</v>
       </c>
       <c r="J30">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K30">
         <v>17</v>
@@ -1867,10 +1867,10 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J31">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K31">
         <v>19</v>
@@ -1902,7 +1902,7 @@
         <v>3</v>
       </c>
       <c r="J32">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K32">
         <v>14</v>
@@ -1934,7 +1934,7 @@
         <v>2</v>
       </c>
       <c r="J33">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K33">
         <v>5</v>
@@ -1957,22 +1957,22 @@
         <v>13</v>
       </c>
       <c r="F34">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G34">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J34">
         <v>75</v>
       </c>
       <c r="K34">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1992,19 +1992,19 @@
         <v>38</v>
       </c>
       <c r="F35">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G35">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J35">
         <v>31</v>
       </c>
       <c r="K35">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2068,7 +2068,7 @@
         <v>13</v>
       </c>
       <c r="J37">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K37">
         <v>13</v>
@@ -2292,7 +2292,7 @@
         <v>4</v>
       </c>
       <c r="J44">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K44">
         <v>6</v>
@@ -2897,7 +2897,7 @@
         <v>13</v>
       </c>
       <c r="F63">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G63">
         <v>2</v>
@@ -2906,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="I63">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J63">
         <v>64</v>
@@ -2976,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="J65">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K65">
         <v>2</v>
@@ -3040,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="J67">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -3497,7 +3497,7 @@
         <v>3</v>
       </c>
       <c r="J81">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K81">
         <v>1</v>
@@ -3800,7 +3800,7 @@
         <v>1</v>
       </c>
       <c r="J90">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -3832,7 +3832,7 @@
         <v>1</v>
       </c>
       <c r="J91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K91">
         <v>1</v>
@@ -4376,7 +4376,7 @@
         <v>87</v>
       </c>
       <c r="G108">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H108">
         <v>1</v>
@@ -4385,10 +4385,10 @@
         <v>16</v>
       </c>
       <c r="J108">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="K108">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -4417,10 +4417,10 @@
         <v>1</v>
       </c>
       <c r="I109">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J109">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K109">
         <v>2</v>
@@ -4507,10 +4507,10 @@
         <v>13</v>
       </c>
       <c r="F112">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G112">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H112">
         <v>1</v>
@@ -4519,10 +4519,10 @@
         <v>9</v>
       </c>
       <c r="J112">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="K112">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
@@ -4734,19 +4734,19 @@
         <v>111</v>
       </c>
       <c r="F119">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="G119">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I119">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J119">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K119">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -4798,19 +4798,19 @@
         <v>113</v>
       </c>
       <c r="F121">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="G121">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I121">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J121">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K121">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
@@ -5310,19 +5310,19 @@
         <v>98</v>
       </c>
       <c r="F137">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="G137">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I137">
         <v>1</v>
       </c>
       <c r="J137">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="K137">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
@@ -5383,10 +5383,10 @@
         <v>1</v>
       </c>
       <c r="I139">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J139">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K139">
         <v>1</v>
@@ -5546,10 +5546,10 @@
         <v>3</v>
       </c>
       <c r="I144">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J144">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K144">
         <v>33</v>
@@ -5584,7 +5584,7 @@
         <v>14</v>
       </c>
       <c r="J145">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K145">
         <v>8</v>
@@ -5680,7 +5680,7 @@
         <v>13</v>
       </c>
       <c r="J148">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K148">
         <v>7</v>
@@ -5712,10 +5712,10 @@
         <v>3</v>
       </c>
       <c r="I149">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J149">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K149">
         <v>8</v>
@@ -5779,10 +5779,10 @@
         <v>1</v>
       </c>
       <c r="I151">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J151">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K151">
         <v>2</v>
@@ -6086,7 +6086,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K160" xr:uid="{93986562-B447-4A8F-B125-FC2B30B194DB}"/>
+  <autoFilter ref="A1:K160" xr:uid="{18236B7C-EAD0-4A33-BAC5-30A8716B0C5A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>